<commit_message>
delta: add new PVs and fix wrong out record type
Add new PVs, based on the most recent delta undulator control interface
and fix some monitor records ('-Mon' suffix) which were using type
analog output, while they should be analog inputs.
</commit_message>
<xml_diff>
--- a/etc/Delta.xlsx
+++ b/etc/Delta.xlsx
@@ -5,24 +5,25 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Delta" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$84</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Delta!$A$1:$K$84</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Delta!$A$1:$K$84</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$84</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="296">
   <si>
     <t xml:space="preserve">Nº</t>
   </si>
@@ -297,6 +298,15 @@
     <t xml:space="preserve">EnFlags[12]</t>
   </si>
   <si>
+    <t xml:space="preserve">Enable Generic Coupling of Axes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnGeneralCoupling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnFlags[13]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Homing acceleration deceleration rate</t>
   </si>
   <si>
@@ -375,6 +385,45 @@
     <t xml:space="preserve">CamTScaling</t>
   </si>
   <si>
+    <t xml:space="preserve">Select Master Axis for General Coupling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingMaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Slave Axis for General Coupling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingSlaves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling Direction of First Slave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingDirection0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingDirection[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling Direction of Second Slave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingDirection1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingDirection[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling Direction of Third Slave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingDirection2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CouplingDirection[2]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Axis A position</t>
   </si>
   <si>
@@ -405,6 +454,27 @@
     <t xml:space="preserve">AxisA.OutputCurrent</t>
   </si>
   <si>
+    <t xml:space="preserve">Axis A position error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisAPositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisA.PositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axis A torque reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisATorqueReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisA.TorqueReference</t>
+  </si>
+  <si>
     <t xml:space="preserve">Axis A status</t>
   </si>
   <si>
@@ -504,6 +574,24 @@
     <t xml:space="preserve">AxisB.OutputCurrent</t>
   </si>
   <si>
+    <t xml:space="preserve">Axis B position error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisBPositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisB.PositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axis B torque reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisB:TorqueReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisB.TorqueReference</t>
+  </si>
+  <si>
     <t xml:space="preserve">Axis B status</t>
   </si>
   <si>
@@ -603,6 +691,24 @@
     <t xml:space="preserve">AxisC.OutputCurrent</t>
   </si>
   <si>
+    <t xml:space="preserve">Axis C position error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisCPositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisC.PositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axis C torque reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisCTorqueReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisC.TorqueReference</t>
+  </si>
+  <si>
     <t xml:space="preserve">Axis C status</t>
   </si>
   <si>
@@ -700,6 +806,24 @@
   </si>
   <si>
     <t xml:space="preserve">AxisD.OutputCurrent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axis D position error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisDPositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisD.PositionError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axis D torque reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisDTorqueReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisD.TorqueReference</t>
   </si>
   <si>
     <t xml:space="preserve">Axis D status</t>
@@ -1169,30 +1293,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:84"/>
+  <dimension ref="1:98"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="237" zoomScaleNormal="237" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H57" activeCellId="0" sqref="H57"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="25.0204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="37.6173469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="5.76020408163265"/>
-    <col collapsed="false" hidden="false" max="1018" min="13" style="8" width="33.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="33.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="1018" min="13" style="8" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="32.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,23 +2302,21 @@
         <v>88</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="F27" s="18" t="str">
         <f aca="false">C27&amp;D27&amp;E27</f>
-        <v>$(P)$(R)HomingAccel-SP</v>
+        <v>$(P)$(R)EnGeneralCoupling-Cmd</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H27" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="19" t="s">
-        <v>91</v>
-      </c>
+      <c r="I27" s="19"/>
       <c r="J27" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K27" s="20" t="s">
         <v>18</v>
@@ -2208,23 +2330,23 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="F28" s="18" t="str">
         <f aca="false">C28&amp;D28&amp;E28</f>
-        <v>$(P)$(R)HomingJerk-SP</v>
+        <v>$(P)$(R)HomingAccel-SP</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H28" s="19" t="s">
         <v>48</v>
@@ -2233,7 +2355,7 @@
         <v>94</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K28" s="20" t="s">
         <v>18</v>
@@ -2256,14 +2378,14 @@
         <v>96</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F29" s="18" t="str">
         <f aca="false">C29&amp;D29&amp;E29</f>
-        <v>$(P)$(R)HomingSpeed-SP</v>
+        <v>$(P)$(R)HomingJerk-SP</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H29" s="19" t="s">
         <v>48</v>
@@ -2295,20 +2417,20 @@
         <v>99</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F30" s="18" t="str">
         <f aca="false">C30&amp;D30&amp;E30</f>
-        <v>$(P)$(R)MoveAccel-SP</v>
+        <v>$(P)$(R)HomingSpeed-SP</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H30" s="19" t="s">
         <v>48</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="J30" s="19" t="s">
         <v>99</v>
@@ -2325,23 +2447,23 @@
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F31" s="18" t="str">
         <f aca="false">C31&amp;D31&amp;E31</f>
-        <v>$(P)$(R)MoveJerk-SP</v>
+        <v>$(P)$(R)MoveAccel-SP</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>48</v>
@@ -2350,7 +2472,7 @@
         <v>94</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K31" s="20" t="s">
         <v>18</v>
@@ -2364,23 +2486,23 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F32" s="18" t="str">
         <f aca="false">C32&amp;D32&amp;E32</f>
-        <v>$(P)$(R)MoveSpeed-SP</v>
+        <v>$(P)$(R)MoveJerk-SP</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>48</v>
@@ -2389,7 +2511,7 @@
         <v>97</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K32" s="20" t="s">
         <v>18</v>
@@ -2403,32 +2525,32 @@
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F33" s="18" t="str">
         <f aca="false">C33&amp;D33&amp;E33</f>
-        <v>$(P)$(R)OvertravelClearDst-SP</v>
+        <v>$(P)$(R)MoveSpeed-SP</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H33" s="19" t="s">
         <v>48</v>
       </c>
       <c r="I33" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" s="19" t="s">
         <v>106</v>
-      </c>
-      <c r="J33" s="19" t="s">
-        <v>105</v>
       </c>
       <c r="K33" s="20" t="s">
         <v>18</v>
@@ -2451,20 +2573,20 @@
         <v>108</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F34" s="18" t="str">
         <f aca="false">C34&amp;D34&amp;E34</f>
-        <v>$(P)$(R)OvertravelClearSpd-SP</v>
+        <v>$(P)$(R)OvertravelClearDst-SP</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>48</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="J34" s="19" t="s">
         <v>108</v>
@@ -2481,30 +2603,32 @@
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F35" s="18" t="str">
         <f aca="false">C35&amp;D35&amp;E35</f>
-        <v>$(P)$(R)CamDScaling-SP</v>
+        <v>$(P)$(R)OvertravelClearSpd-SP</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H35" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I35" s="19"/>
+      <c r="I35" s="19" t="s">
+        <v>100</v>
+      </c>
       <c r="J35" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K35" s="20" t="s">
         <v>18</v>
@@ -2518,30 +2642,30 @@
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F36" s="18" t="str">
         <f aca="false">C36&amp;D36&amp;E36</f>
-        <v>$(P)$(R)CamTScaling-SP</v>
+        <v>$(P)$(R)CamDScaling-SP</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H36" s="19" t="s">
         <v>48</v>
       </c>
       <c r="I36" s="19"/>
       <c r="J36" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K36" s="20" t="s">
         <v>18</v>
@@ -2555,30 +2679,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F37" s="18" t="str">
         <f aca="false">C37&amp;D37&amp;E37</f>
-        <v>$(P)$(R)AxisAActualPosition-Mon</v>
+        <v>$(P)$(R)CamTScaling-SP</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H37" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I37" s="19" t="s">
-        <v>106</v>
-      </c>
+      <c r="I37" s="19"/>
       <c r="J37" s="19" t="s">
         <v>115</v>
       </c>
@@ -2603,23 +2725,21 @@
         <v>117</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F38" s="18" t="str">
         <f aca="false">C38&amp;D38&amp;E38</f>
-        <v>$(P)$(R)AxisAActualVelocity-Mon</v>
+        <v>$(P)$(R)CouplingMaster-SP</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H38" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I38" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="I38" s="19"/>
       <c r="J38" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K38" s="20" t="s">
         <v>18</v>
@@ -2633,32 +2753,30 @@
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>120</v>
-      </c>
       <c r="E39" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F39" s="18" t="str">
         <f aca="false">C39&amp;D39&amp;E39</f>
-        <v>$(P)$(R)AxisAOutputCurrent-Mon</v>
+        <v>$(P)$(R)CouplingSlaves-SP</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H39" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I39" s="19" t="s">
-        <v>121</v>
-      </c>
+      <c r="I39" s="19"/>
       <c r="J39" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K39" s="20" t="s">
         <v>18</v>
@@ -2672,32 +2790,30 @@
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F40" s="18" t="str">
         <f aca="false">C40&amp;D40&amp;E40</f>
-        <v>$(P)$(R)AxisAAxisStatus-Mon</v>
+        <v>$(P)$(R)CouplingDirection0-SP</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H40" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I40" s="19" t="s">
-        <v>121</v>
-      </c>
+      <c r="I40" s="19"/>
       <c r="J40" s="19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K40" s="20" t="s">
         <v>18</v>
@@ -2711,32 +2827,30 @@
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F41" s="18" t="str">
         <f aca="false">C41&amp;D41&amp;E41</f>
-        <v>$(P)$(R)AxisAMotionStatus-Mon</v>
+        <v>$(P)$(R)CouplingDirection1-SP</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H41" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I41" s="19" t="s">
-        <v>121</v>
-      </c>
+      <c r="I41" s="19"/>
       <c r="J41" s="19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K41" s="20" t="s">
         <v>18</v>
@@ -2750,30 +2864,30 @@
         <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F42" s="18" t="str">
         <f aca="false">C42&amp;D42&amp;E42</f>
-        <v>$(P)$(R)AxisAMoveStatus-Mon</v>
+        <v>$(P)$(R)CouplingDirection2-SP</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="I42" s="19"/>
       <c r="J42" s="19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K42" s="20" t="s">
         <v>18</v>
@@ -2787,30 +2901,32 @@
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E43" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="18" t="str">
         <f aca="false">C43&amp;D43&amp;E43</f>
-        <v>$(P)$(R)AxisADriveEnableStatus-Mon</v>
+        <v>$(P)$(R)AxisAActualPosition-Mon</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H43" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I43" s="19"/>
+      <c r="I43" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J43" s="19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K43" s="20" t="s">
         <v>18</v>
@@ -2824,30 +2940,32 @@
         <v>43</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F44" s="18" t="str">
         <f aca="false">C44&amp;D44&amp;E44</f>
-        <v>$(P)$(R)AxisABrakeStatus-Mon</v>
+        <v>$(P)$(R)AxisAActualVelocity-Mon</v>
       </c>
       <c r="G44" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H44" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="19"/>
+      <c r="I44" s="19" t="s">
+        <v>100</v>
+      </c>
       <c r="J44" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K44" s="20" t="s">
         <v>18</v>
@@ -2861,32 +2979,32 @@
         <v>44</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F45" s="18" t="str">
         <f aca="false">C45&amp;D45&amp;E45</f>
-        <v>$(P)$(R)AxisAHomePos-SP</v>
+        <v>$(P)$(R)AxisAOutputCurrent-Mon</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K45" s="20" t="s">
         <v>18</v>
@@ -2900,30 +3018,32 @@
         <v>45</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="F46" s="18" t="str">
         <f aca="false">C46&amp;D46&amp;E46</f>
-        <v>$(P)$(R)AxisAMove-Sel</v>
+        <v>$(P)$(R)AxisAPositionError-Mon</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I46" s="19"/>
+        <v>17</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J46" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K46" s="20" t="s">
         <v>18</v>
@@ -2937,32 +3057,32 @@
         <v>46</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F47" s="18" t="str">
         <f aca="false">C47&amp;D47&amp;E47</f>
-        <v>$(P)$(R)AxisAMovePos-SP</v>
+        <v>$(P)$(R)AxisATorqueReference-Mon</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K47" s="20" t="s">
         <v>18</v>
@@ -2976,32 +3096,32 @@
         <v>47</v>
       </c>
       <c r="B48" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="16" t="s">
         <v>147</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>148</v>
       </c>
       <c r="E48" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="18" t="str">
         <f aca="false">C48&amp;D48&amp;E48</f>
-        <v>$(P)$(R)AxisBActualPosition-Mon</v>
+        <v>$(P)$(R)AxisAAxisStatus-Mon</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K48" s="20" t="s">
         <v>18</v>
@@ -3015,32 +3135,32 @@
         <v>48</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="16" t="s">
         <v>150</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>151</v>
       </c>
       <c r="E49" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F49" s="18" t="str">
         <f aca="false">C49&amp;D49&amp;E49</f>
-        <v>$(P)$(R)AxisBActualVelocity-Mon</v>
+        <v>$(P)$(R)AxisAMotionStatus-Mon</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K49" s="20" t="s">
         <v>18</v>
@@ -3054,32 +3174,30 @@
         <v>49</v>
       </c>
       <c r="B50" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>154</v>
       </c>
       <c r="E50" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F50" s="18" t="str">
         <f aca="false">C50&amp;D50&amp;E50</f>
-        <v>$(P)$(R)AxisBOutputCurrent-Mon</v>
+        <v>$(P)$(R)AxisAMoveStatus-Mon</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H50" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I50" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I50" s="19"/>
       <c r="J50" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K50" s="20" t="s">
         <v>18</v>
@@ -3093,32 +3211,30 @@
         <v>50</v>
       </c>
       <c r="B51" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>157</v>
       </c>
       <c r="E51" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F51" s="18" t="str">
         <f aca="false">C51&amp;D51&amp;E51</f>
-        <v>$(P)$(R)AxisBAxisStatus-Mon</v>
+        <v>$(P)$(R)AxisADriveEnableStatus-Mon</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I51" s="19"/>
       <c r="J51" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K51" s="20" t="s">
         <v>18</v>
@@ -3132,32 +3248,30 @@
         <v>51</v>
       </c>
       <c r="B52" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="16" t="s">
         <v>159</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>160</v>
       </c>
       <c r="E52" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F52" s="18" t="str">
         <f aca="false">C52&amp;D52&amp;E52</f>
-        <v>$(P)$(R)AxisBMotionStatus-Mon</v>
+        <v>$(P)$(R)AxisABrakeStatus-Mon</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I52" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I52" s="19"/>
       <c r="J52" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K52" s="20" t="s">
         <v>18</v>
@@ -3171,30 +3285,32 @@
         <v>52</v>
       </c>
       <c r="B53" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="C53" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>163</v>
-      </c>
       <c r="E53" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F53" s="18" t="str">
         <f aca="false">C53&amp;D53&amp;E53</f>
-        <v>$(P)$(R)AxisBMoveStatus-Mon</v>
+        <v>$(P)$(R)AxisAHomePos-SP</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" s="19"/>
+        <v>48</v>
+      </c>
+      <c r="I53" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J53" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K53" s="20" t="s">
         <v>18</v>
@@ -3208,30 +3324,30 @@
         <v>53</v>
       </c>
       <c r="B54" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="C54" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>166</v>
-      </c>
       <c r="E54" s="17" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="F54" s="18" t="str">
         <f aca="false">C54&amp;D54&amp;E54</f>
-        <v>$(P)$(R)AxisBDriveEnableStatus-Mon</v>
+        <v>$(P)$(R)AxisAMove-Sel</v>
       </c>
       <c r="G54" s="19" t="s">
         <v>16</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="I54" s="19"/>
       <c r="J54" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K54" s="20" t="s">
         <v>18</v>
@@ -3245,30 +3361,32 @@
         <v>54</v>
       </c>
       <c r="B55" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="C55" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>169</v>
-      </c>
       <c r="E55" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F55" s="18" t="str">
         <f aca="false">C55&amp;D55&amp;E55</f>
-        <v>$(P)$(R)AxisBBrakeStatus-Mon</v>
+        <v>$(P)$(R)AxisAMovePos-SP</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I55" s="19"/>
+        <v>48</v>
+      </c>
+      <c r="I55" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J55" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K55" s="20" t="s">
         <v>18</v>
@@ -3282,32 +3400,32 @@
         <v>55</v>
       </c>
       <c r="B56" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="C56" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>172</v>
-      </c>
       <c r="E56" s="17" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F56" s="18" t="str">
         <f aca="false">C56&amp;D56&amp;E56</f>
-        <v>$(P)$(R)AxisBHomePos-SP</v>
+        <v>$(P)$(R)AxisBActualPosition-Mon</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K56" s="20" t="s">
         <v>18</v>
@@ -3321,30 +3439,32 @@
         <v>56</v>
       </c>
       <c r="B57" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="C57" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>175</v>
-      </c>
       <c r="E57" s="17" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="F57" s="18" t="str">
         <f aca="false">C57&amp;D57&amp;E57</f>
-        <v>$(P)$(R)AxisBMove-Sel</v>
+        <v>$(P)$(R)AxisBActualVelocity-Mon</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I57" s="19"/>
+        <v>17</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>100</v>
+      </c>
       <c r="J57" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K57" s="20" t="s">
         <v>18</v>
@@ -3358,32 +3478,32 @@
         <v>57</v>
       </c>
       <c r="B58" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="C58" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>178</v>
-      </c>
       <c r="E58" s="17" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F58" s="18" t="str">
         <f aca="false">C58&amp;D58&amp;E58</f>
-        <v>$(P)$(R)AxisBMovePos-SP</v>
+        <v>$(P)$(R)AxisBOutputCurrent-Mon</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H58" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K58" s="20" t="s">
         <v>18</v>
@@ -3397,32 +3517,32 @@
         <v>58</v>
       </c>
       <c r="B59" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>181</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F59" s="18" t="str">
         <f aca="false">C59&amp;D59&amp;E59</f>
-        <v>$(P)$(R)AxisCActualPosition-Mon</v>
+        <v>$(P)$(R)AxisBPositionError-Mon</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H59" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K59" s="20" t="s">
         <v>18</v>
@@ -3436,32 +3556,32 @@
         <v>59</v>
       </c>
       <c r="B60" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>184</v>
       </c>
       <c r="E60" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F60" s="18" t="str">
         <f aca="false">C60&amp;D60&amp;E60</f>
-        <v>$(P)$(R)AxisCActualVelocity-Mon</v>
+        <v>$(P)$(R)AxisB:TorqueReference-Mon</v>
       </c>
       <c r="G60" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I60" s="19" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K60" s="20" t="s">
         <v>18</v>
@@ -3475,32 +3595,32 @@
         <v>60</v>
       </c>
       <c r="B61" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="16" t="s">
         <v>186</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>187</v>
       </c>
       <c r="E61" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F61" s="18" t="str">
         <f aca="false">C61&amp;D61&amp;E61</f>
-        <v>$(P)$(R)AxisCOutputCurrent-Mon</v>
+        <v>$(P)$(R)AxisBAxisStatus-Mon</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H61" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K61" s="20" t="s">
         <v>18</v>
@@ -3514,32 +3634,32 @@
         <v>61</v>
       </c>
       <c r="B62" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="16" t="s">
         <v>189</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="16" t="s">
-        <v>190</v>
       </c>
       <c r="E62" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F62" s="18" t="str">
         <f aca="false">C62&amp;D62&amp;E62</f>
-        <v>$(P)$(R)AxisCAxisStatus-Mon</v>
+        <v>$(P)$(R)AxisBMotionStatus-Mon</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I62" s="19" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K62" s="20" t="s">
         <v>18</v>
@@ -3553,32 +3673,30 @@
         <v>62</v>
       </c>
       <c r="B63" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="16" t="s">
         <v>192</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="16" t="s">
-        <v>193</v>
       </c>
       <c r="E63" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F63" s="18" t="str">
         <f aca="false">C63&amp;D63&amp;E63</f>
-        <v>$(P)$(R)AxisCMotionStatus-Mon</v>
+        <v>$(P)$(R)AxisBMoveStatus-Mon</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I63" s="19" t="s">
-        <v>121</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I63" s="19"/>
       <c r="J63" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K63" s="20" t="s">
         <v>18</v>
@@ -3592,20 +3710,20 @@
         <v>63</v>
       </c>
       <c r="B64" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="16" t="s">
         <v>195</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>196</v>
       </c>
       <c r="E64" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F64" s="18" t="str">
         <f aca="false">C64&amp;D64&amp;E64</f>
-        <v>$(P)$(R)AxisCMoveStatus-Mon</v>
+        <v>$(P)$(R)AxisBDriveEnableStatus-Mon</v>
       </c>
       <c r="G64" s="19" t="s">
         <v>16</v>
@@ -3615,7 +3733,7 @@
       </c>
       <c r="I64" s="19"/>
       <c r="J64" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K64" s="20" t="s">
         <v>18</v>
@@ -3629,20 +3747,20 @@
         <v>64</v>
       </c>
       <c r="B65" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="16" t="s">
         <v>198</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>199</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F65" s="18" t="str">
         <f aca="false">C65&amp;D65&amp;E65</f>
-        <v>$(P)$(R)AxisCDriveEnableStatus-Mon</v>
+        <v>$(P)$(R)AxisBBrakeStatus-Mon</v>
       </c>
       <c r="G65" s="19" t="s">
         <v>16</v>
@@ -3652,7 +3770,7 @@
       </c>
       <c r="I65" s="19"/>
       <c r="J65" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K65" s="20" t="s">
         <v>18</v>
@@ -3666,30 +3784,32 @@
         <v>65</v>
       </c>
       <c r="B66" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="C66" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="16" t="s">
-        <v>202</v>
-      </c>
       <c r="E66" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F66" s="18" t="str">
         <f aca="false">C66&amp;D66&amp;E66</f>
-        <v>$(P)$(R)AxisCBrakeStatus-Mon</v>
+        <v>$(P)$(R)AxisBHomePos-SP</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H66" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I66" s="19"/>
+        <v>48</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J66" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K66" s="20" t="s">
         <v>18</v>
@@ -3703,32 +3823,30 @@
         <v>66</v>
       </c>
       <c r="B67" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="C67" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="16" t="s">
-        <v>205</v>
-      </c>
       <c r="E67" s="17" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="F67" s="18" t="str">
         <f aca="false">C67&amp;D67&amp;E67</f>
-        <v>$(P)$(R)AxisCHomePos-SP</v>
+        <v>$(P)$(R)AxisBMove-Sel</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H67" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I67" s="19" t="s">
-        <v>106</v>
-      </c>
+      <c r="I67" s="19"/>
       <c r="J67" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K67" s="20" t="s">
         <v>18</v>
@@ -3742,30 +3860,32 @@
         <v>67</v>
       </c>
       <c r="B68" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C68" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D68" s="16" t="s">
-        <v>208</v>
-      </c>
       <c r="E68" s="17" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="F68" s="18" t="str">
         <f aca="false">C68&amp;D68&amp;E68</f>
-        <v>$(P)$(R)AxisCMove-Sel</v>
+        <v>$(P)$(R)AxisBMovePos-SP</v>
       </c>
       <c r="G68" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H68" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I68" s="19"/>
+      <c r="I68" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J68" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K68" s="20" t="s">
         <v>18</v>
@@ -3779,32 +3899,32 @@
         <v>68</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C69" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>211</v>
-      </c>
       <c r="E69" s="17" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F69" s="18" t="str">
         <f aca="false">C69&amp;D69&amp;E69</f>
-        <v>$(P)$(R)AxisCMovePos-SP</v>
+        <v>$(P)$(R)AxisCActualPosition-Mon</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I69" s="19" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J69" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K69" s="20" t="s">
         <v>18</v>
@@ -3818,32 +3938,32 @@
         <v>69</v>
       </c>
       <c r="B70" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="16" t="s">
         <v>213</v>
-      </c>
-      <c r="C70" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="16" t="s">
-        <v>214</v>
       </c>
       <c r="E70" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F70" s="18" t="str">
         <f aca="false">C70&amp;D70&amp;E70</f>
-        <v>$(P)$(R)AxisDActualPosition-Mon</v>
+        <v>$(P)$(R)AxisCActualVelocity-Mon</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H70" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I70" s="19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J70" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K70" s="20" t="s">
         <v>18</v>
@@ -3857,32 +3977,32 @@
         <v>70</v>
       </c>
       <c r="B71" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="16" t="s">
         <v>216</v>
-      </c>
-      <c r="C71" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="16" t="s">
-        <v>217</v>
       </c>
       <c r="E71" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F71" s="18" t="str">
         <f aca="false">C71&amp;D71&amp;E71</f>
-        <v>$(P)$(R)AxisDActualVelocity-Mon</v>
+        <v>$(P)$(R)AxisCOutputCurrent-Mon</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H71" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I71" s="19" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="J71" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K71" s="20" t="s">
         <v>18</v>
@@ -3896,32 +4016,32 @@
         <v>71</v>
       </c>
       <c r="B72" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="16" t="s">
         <v>219</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="16" t="s">
-        <v>220</v>
       </c>
       <c r="E72" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F72" s="18" t="str">
         <f aca="false">C72&amp;D72&amp;E72</f>
-        <v>$(P)$(R)AxisDOutputCurrent-Mon</v>
+        <v>$(P)$(R)AxisCPositionError-Mon</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H72" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="J72" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K72" s="20" t="s">
         <v>18</v>
@@ -3935,32 +4055,32 @@
         <v>72</v>
       </c>
       <c r="B73" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="16" t="s">
         <v>222</v>
-      </c>
-      <c r="C73" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="16" t="s">
-        <v>223</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F73" s="18" t="str">
         <f aca="false">C73&amp;D73&amp;E73</f>
-        <v>$(P)$(R)AxisDAxisStatus-Mon</v>
+        <v>$(P)$(R)AxisCTorqueReference-Mon</v>
       </c>
       <c r="G73" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H73" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I73" s="19" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="J73" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K73" s="20" t="s">
         <v>18</v>
@@ -3974,32 +4094,32 @@
         <v>73</v>
       </c>
       <c r="B74" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="16" t="s">
         <v>225</v>
-      </c>
-      <c r="C74" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="16" t="s">
-        <v>226</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F74" s="18" t="str">
         <f aca="false">C74&amp;D74&amp;E74</f>
-        <v>$(P)$(R)AxisDMotionStatus-Mon</v>
+        <v>$(P)$(R)AxisCAxisStatus-Mon</v>
       </c>
       <c r="G74" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H74" s="19" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I74" s="19" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="J74" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K74" s="20" t="s">
         <v>18</v>
@@ -4013,30 +4133,32 @@
         <v>74</v>
       </c>
       <c r="B75" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="16" t="s">
         <v>228</v>
-      </c>
-      <c r="C75" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="16" t="s">
-        <v>229</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F75" s="18" t="str">
         <f aca="false">C75&amp;D75&amp;E75</f>
-        <v>$(P)$(R)AxisDMoveStatus-Mon</v>
+        <v>$(P)$(R)AxisCMotionStatus-Mon</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H75" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I75" s="19"/>
+      <c r="I75" s="19" t="s">
+        <v>137</v>
+      </c>
       <c r="J75" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K75" s="20" t="s">
         <v>18</v>
@@ -4050,20 +4172,20 @@
         <v>75</v>
       </c>
       <c r="B76" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="16" t="s">
         <v>231</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="16" t="s">
-        <v>232</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F76" s="18" t="str">
         <f aca="false">C76&amp;D76&amp;E76</f>
-        <v>$(P)$(R)AxisDDriveEnableStatus-Mon</v>
+        <v>$(P)$(R)AxisCMoveStatus-Mon</v>
       </c>
       <c r="G76" s="19" t="s">
         <v>16</v>
@@ -4073,7 +4195,7 @@
       </c>
       <c r="I76" s="19"/>
       <c r="J76" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K76" s="20" t="s">
         <v>18</v>
@@ -4087,20 +4209,20 @@
         <v>76</v>
       </c>
       <c r="B77" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="16" t="s">
         <v>234</v>
-      </c>
-      <c r="C77" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D77" s="16" t="s">
-        <v>235</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F77" s="18" t="str">
         <f aca="false">C77&amp;D77&amp;E77</f>
-        <v>$(P)$(R)AxisDBrakeStatus-Mon</v>
+        <v>$(P)$(R)AxisCDriveEnableStatus-Mon</v>
       </c>
       <c r="G77" s="19" t="s">
         <v>16</v>
@@ -4110,7 +4232,7 @@
       </c>
       <c r="I77" s="19"/>
       <c r="J77" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K77" s="20" t="s">
         <v>18</v>
@@ -4124,32 +4246,30 @@
         <v>77</v>
       </c>
       <c r="B78" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C78" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="C78" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" s="16" t="s">
-        <v>238</v>
-      </c>
       <c r="E78" s="17" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F78" s="18" t="str">
         <f aca="false">C78&amp;D78&amp;E78</f>
-        <v>$(P)$(R)AxisDHomePos-SP</v>
+        <v>$(P)$(R)AxisCBrakeStatus-Mon</v>
       </c>
       <c r="G78" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H78" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I78" s="19" t="s">
-        <v>106</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I78" s="19"/>
       <c r="J78" s="19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K78" s="20" t="s">
         <v>18</v>
@@ -4163,30 +4283,32 @@
         <v>78</v>
       </c>
       <c r="B79" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="C79" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>241</v>
-      </c>
       <c r="E79" s="17" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="F79" s="18" t="str">
         <f aca="false">C79&amp;D79&amp;E79</f>
-        <v>$(P)$(R)AxisDMove-Sel</v>
+        <v>$(P)$(R)AxisCHomePos-SP</v>
       </c>
       <c r="G79" s="19" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H79" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I79" s="19"/>
+      <c r="I79" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J79" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K79" s="20" t="s">
         <v>18</v>
@@ -4200,32 +4322,30 @@
         <v>79</v>
       </c>
       <c r="B80" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="C80" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>244</v>
-      </c>
       <c r="E80" s="17" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="F80" s="18" t="str">
         <f aca="false">C80&amp;D80&amp;E80</f>
-        <v>$(P)$(R)AxisDMovePos-SP</v>
+        <v>$(P)$(R)AxisCMove-Sel</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="H80" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I80" s="19" t="s">
-        <v>106</v>
-      </c>
+      <c r="I80" s="19"/>
       <c r="J80" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K80" s="20" t="s">
         <v>18</v>
@@ -4239,28 +4359,30 @@
         <v>80</v>
       </c>
       <c r="B81" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="C81" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D81" s="16" t="s">
-        <v>247</v>
-      </c>
       <c r="E81" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F81" s="18" t="str">
         <f aca="false">C81&amp;D81&amp;E81</f>
-        <v>$(P)$(R)RunFlag-Mon</v>
+        <v>$(P)$(R)AxisCMovePos-SP</v>
       </c>
       <c r="G81" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H81" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I81" s="19"/>
+        <v>48</v>
+      </c>
+      <c r="I81" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J81" s="19" t="s">
         <v>247</v>
       </c>
@@ -4289,17 +4411,19 @@
       </c>
       <c r="F82" s="18" t="str">
         <f aca="false">C82&amp;D82&amp;E82</f>
-        <v>$(P)$(R)ControllerStatus-Mon</v>
+        <v>$(P)$(R)AxisDActualPosition-Mon</v>
       </c>
       <c r="G82" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H82" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I82" s="19"/>
+      <c r="I82" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="J82" s="19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K82" s="20" t="s">
         <v>18</v>
@@ -4313,30 +4437,32 @@
         <v>82</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C83" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D83" s="16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E83" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F83" s="18" t="str">
         <f aca="false">C83&amp;D83&amp;E83</f>
-        <v>$(P)$(R)AxisFault-Mon</v>
+        <v>$(P)$(R)AxisDActualVelocity-Mon</v>
       </c>
       <c r="G83" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H83" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I83" s="19"/>
+      <c r="I83" s="19" t="s">
+        <v>100</v>
+      </c>
       <c r="J83" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="K83" s="20" t="s">
         <v>18</v>
@@ -4350,40 +4476,572 @@
         <v>83</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C84" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E84" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F84" s="18" t="str">
         <f aca="false">C84&amp;D84&amp;E84</f>
+        <v>$(P)$(R)AxisDOutputCurrent-Mon</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H84" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I84" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="J84" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="K84" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L84" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="14" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" s="18" t="str">
+        <f aca="false">C85&amp;D85&amp;E85</f>
+        <v>$(P)$(R)AxisDPositionError-Mon</v>
+      </c>
+      <c r="G85" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H85" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I85" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J85" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="K85" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L85" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="14" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86" s="18" t="str">
+        <f aca="false">C86&amp;D86&amp;E86</f>
+        <v>$(P)$(R)AxisDTorqueReference-Mon</v>
+      </c>
+      <c r="G86" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H86" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I86" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="J86" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="K86" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L86" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="14" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C87" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F87" s="18" t="str">
+        <f aca="false">C87&amp;D87&amp;E87</f>
+        <v>$(P)$(R)AxisDAxisStatus-Mon</v>
+      </c>
+      <c r="G87" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H87" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I87" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="J87" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="K87" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L87" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="14" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C88" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="E88" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" s="18" t="str">
+        <f aca="false">C88&amp;D88&amp;E88</f>
+        <v>$(P)$(R)AxisDMotionStatus-Mon</v>
+      </c>
+      <c r="G88" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H88" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I88" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="J88" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="K88" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L88" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="14" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="E89" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F89" s="18" t="str">
+        <f aca="false">C89&amp;D89&amp;E89</f>
+        <v>$(P)$(R)AxisDMoveStatus-Mon</v>
+      </c>
+      <c r="G89" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I89" s="19"/>
+      <c r="J89" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="K89" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L89" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="14" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C90" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="E90" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90" s="18" t="str">
+        <f aca="false">C90&amp;D90&amp;E90</f>
+        <v>$(P)$(R)AxisDDriveEnableStatus-Mon</v>
+      </c>
+      <c r="G90" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H90" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I90" s="19"/>
+      <c r="J90" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="K90" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L90" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="14" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="E91" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F91" s="18" t="str">
+        <f aca="false">C91&amp;D91&amp;E91</f>
+        <v>$(P)$(R)AxisDBrakeStatus-Mon</v>
+      </c>
+      <c r="G91" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H91" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I91" s="19"/>
+      <c r="J91" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="K91" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L91" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="14" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="C92" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="E92" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F92" s="18" t="str">
+        <f aca="false">C92&amp;D92&amp;E92</f>
+        <v>$(P)$(R)AxisDHomePos-SP</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H92" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I92" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J92" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="K92" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L92" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="14" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="E93" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F93" s="18" t="str">
+        <f aca="false">C93&amp;D93&amp;E93</f>
+        <v>$(P)$(R)AxisDMove-Sel</v>
+      </c>
+      <c r="G93" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H93" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I93" s="19"/>
+      <c r="J93" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="K93" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L93" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="14" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F94" s="18" t="str">
+        <f aca="false">C94&amp;D94&amp;E94</f>
+        <v>$(P)$(R)AxisDMovePos-SP</v>
+      </c>
+      <c r="G94" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H94" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I94" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J94" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="K94" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L94" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="14" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="E95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F95" s="18" t="str">
+        <f aca="false">C95&amp;D95&amp;E95</f>
+        <v>$(P)$(R)RunFlag-Mon</v>
+      </c>
+      <c r="G95" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H95" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I95" s="19"/>
+      <c r="J95" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="K95" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L95" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="14" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="E96" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96" s="18" t="str">
+        <f aca="false">C96&amp;D96&amp;E96</f>
+        <v>$(P)$(R)ControllerStatus-Mon</v>
+      </c>
+      <c r="G96" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H96" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I96" s="19"/>
+      <c r="J96" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="K96" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L96" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="14" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="E97" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F97" s="18" t="str">
+        <f aca="false">C97&amp;D97&amp;E97</f>
+        <v>$(P)$(R)AxisFault-Mon</v>
+      </c>
+      <c r="G97" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H97" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I97" s="19"/>
+      <c r="J97" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="K97" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L97" s="19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="14" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C98" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="E98" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" s="18" t="str">
+        <f aca="false">C98&amp;D98&amp;E98</f>
         <v>$(P)$(R)LastOpSuccessful-Mon</v>
       </c>
-      <c r="G84" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="H84" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I84" s="19"/>
-      <c r="J84" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="K84" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="L84" s="19" t="n">
+      <c r="G98" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H98" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I98" s="19"/>
+      <c r="J98" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="K98" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L98" s="19" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K84"/>
+  <autoFilter ref="A1:K1"/>
   <conditionalFormatting sqref="B3">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(B3)&gt;40</formula>
@@ -4434,338 +5092,338 @@
       <formula>LEN(B13)&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B58">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:B68">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B49)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B57)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B59)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B69)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:B69">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70:B81">
     <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B60)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B70)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
     <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B70)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B82)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B80">
+      <formula>LEN(B83)&gt;40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B94">
     <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(B71)&gt;40</formula>
+      <formula>LEN(B83)&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1:E84" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1:E98" type="list">
       <formula1>"-Mon,-Sel,-Sts,-SP,-RB,-Cmd"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
delta: Fix typo in Delta reference spreadsheet
Fix Torque reference PV name for Axis B.
It was, incorrectly, named as *AxisB:TorqueReference*, when
it should be *AxisBTorqueReference*.
</commit_message>
<xml_diff>
--- a/etc/Delta.xlsx
+++ b/etc/Delta.xlsx
@@ -11,19 +11,20 @@
     <sheet name="Delta" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$98</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -586,7 +587,7 @@
     <t xml:space="preserve">Axis B torque reference</t>
   </si>
   <si>
-    <t xml:space="preserve">AxisB:TorqueReference</t>
+    <t xml:space="preserve">AxisBTorqueReference</t>
   </si>
   <si>
     <t xml:space="preserve">AxisB.TorqueReference</t>
@@ -1295,28 +1296,28 @@
   </sheetPr>
   <dimension ref="1:98"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="1018" min="13" style="8" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="1018" min="13" style="8" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,7 +3570,7 @@
       </c>
       <c r="F60" s="18" t="str">
         <f aca="false">C60&amp;D60&amp;E60</f>
-        <v>$(P)$(R)AxisB:TorqueReference-Mon</v>
+        <v>$(P)$(R)AxisBTorqueReference-Mon</v>
       </c>
       <c r="G60" s="19" t="s">
         <v>93</v>
@@ -5041,7 +5042,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1"/>
+  <autoFilter ref="A1:K98"/>
   <conditionalFormatting sqref="B3">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(B3)&gt;40</formula>

</xml_diff>